<commit_message>
Update dept(edit, log), rank(edit, log), staff(add, edit, log)
</commit_message>
<xml_diff>
--- a/2.Design/schema.xlsx
+++ b/2.Design/schema.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="107">
   <si>
     <t>rank</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -393,6 +393,66 @@
 야근일자
 야근시간
 야근사유</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>attendance_log</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>what</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reason</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사원번호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>무엇을</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떻게</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>왜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>언제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 아이디</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all_log</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -888,7 +948,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -928,6 +988,39 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -946,12 +1039,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -961,32 +1048,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="2" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1284,10 +1350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E49"/>
+  <dimension ref="B1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1300,12 +1366,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="2" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="7" t="s">
@@ -1349,12 +1415,12 @@
     </row>
     <row r="6" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="7" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="7" t="s">
@@ -1398,12 +1464,12 @@
     </row>
     <row r="11" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="12" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="7" t="s">
@@ -1535,12 +1601,12 @@
     </row>
     <row r="23" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="24" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="7" t="s">
@@ -1628,7 +1694,7 @@
         <v>63</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="13" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1640,128 +1706,128 @@
         <v>65</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="34" spans="2:5" hidden="1">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="23"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="32"/>
     </row>
     <row r="35" spans="2:5" hidden="1">
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" spans="2:5" hidden="1">
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E36" s="20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="37" spans="2:5" hidden="1">
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E37" s="29" t="s">
+      <c r="E37" s="20" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="38" spans="2:5" hidden="1">
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="29" t="s">
+      <c r="D38" s="19"/>
+      <c r="E38" s="20" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="39" spans="2:5" hidden="1">
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="29" t="s">
+      <c r="D39" s="19"/>
+      <c r="E39" s="20" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="40" spans="2:5" hidden="1">
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="28"/>
-      <c r="E40" s="29" t="s">
+      <c r="D40" s="19"/>
+      <c r="E40" s="20" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="41" spans="2:5" hidden="1">
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D41" s="28"/>
-      <c r="E41" s="29" t="s">
+      <c r="D41" s="19"/>
+      <c r="E41" s="20" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="17.25" hidden="1" thickBot="1">
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="C42" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="32" t="s">
+      <c r="D42" s="22"/>
+      <c r="E42" s="23" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="44" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="18"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="29"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="7" t="s">
@@ -1829,8 +1895,235 @@
         <v>54</v>
       </c>
     </row>
+    <row r="50" spans="2:5" ht="17.25" thickBot="1"/>
+    <row r="51" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B51" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="26"/>
+    </row>
+    <row r="52" spans="2:5">
+      <c r="B52" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
+      <c r="B53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="B54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B58" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="34"/>
+    </row>
+    <row r="60" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B60" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="26"/>
+    </row>
+    <row r="61" spans="2:5">
+      <c r="B61" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5">
+      <c r="B63" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5">
+      <c r="B64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B69" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D69" s="5"/>
+      <c r="E69" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B51:E51"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B12:E12"/>

</xml_diff>

<commit_message>
UI, staff, admin, attendance update
</commit_message>
<xml_diff>
--- a/2.Design/schema.xlsx
+++ b/2.Design/schema.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="135">
   <si>
     <t>rank</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -453,6 +453,118 @@
   </si>
   <si>
     <t>log</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rank</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>야근 형태</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reason</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>proxy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사유</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대리자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>비상연락망</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>approval_step</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_step</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>총 결재 단계</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 결재 단계</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신청일자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>시작 날짜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>끝 날짜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(max)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vacation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>휴가 종류</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>overtime_date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>overtime_time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>소속 부서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>야근 날짜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>야근 시간</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1021,6 +1133,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="2" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1047,12 +1165,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1350,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E69"/>
+  <dimension ref="B1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1366,12 +1478,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="2" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="7" t="s">
@@ -1415,12 +1527,12 @@
     </row>
     <row r="6" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="7" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="7" t="s">
@@ -1464,12 +1576,12 @@
     </row>
     <row r="11" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="12" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="7" t="s">
@@ -1601,12 +1713,12 @@
     </row>
     <row r="23" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="24" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="7" t="s">
@@ -1711,12 +1823,12 @@
       </c>
     </row>
     <row r="34" spans="2:5" hidden="1">
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="32"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="34"/>
     </row>
     <row r="35" spans="2:5" hidden="1">
       <c r="B35" s="15" t="s">
@@ -1822,12 +1934,12 @@
     </row>
     <row r="43" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="44" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="29"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="31"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="7" t="s">
@@ -1897,12 +2009,12 @@
     </row>
     <row r="50" spans="2:5" ht="17.25" thickBot="1"/>
     <row r="51" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="26"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="28"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="7" t="s">
@@ -1993,18 +2105,18 @@
       </c>
     </row>
     <row r="59" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="34"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="25"/>
     </row>
     <row r="60" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B60" s="24" t="s">
+      <c r="B60" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="26"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="28"/>
     </row>
     <row r="61" spans="2:5">
       <c r="B61" s="7" t="s">
@@ -2120,8 +2232,512 @@
         <v>100</v>
       </c>
     </row>
+    <row r="70" spans="2:5" ht="17.25" thickBot="1"/>
+    <row r="71" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B71" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="28"/>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5">
+      <c r="B73" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5">
+      <c r="B74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5">
+      <c r="B75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5">
+      <c r="B76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5">
+      <c r="B77" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5">
+      <c r="B78" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5">
+      <c r="B79" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5">
+      <c r="B80" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5">
+      <c r="B81" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5">
+      <c r="B82" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5">
+      <c r="B83" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5">
+      <c r="B84" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5">
+      <c r="B85" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B86" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="5"/>
+      <c r="E86" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="17.25" thickBot="1"/>
+    <row r="88" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B88" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="28"/>
+    </row>
+    <row r="89" spans="2:5">
+      <c r="B89" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5">
+      <c r="B90" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5">
+      <c r="B91" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5">
+      <c r="B92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5">
+      <c r="B93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5">
+      <c r="B94" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5">
+      <c r="B95" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5">
+      <c r="B96" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5">
+      <c r="B97" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5">
+      <c r="B98" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5">
+      <c r="B99" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5">
+      <c r="B100" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5">
+      <c r="B101" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B102" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D102" s="5"/>
+      <c r="E102" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" ht="17.25" thickBot="1"/>
+    <row r="104" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B104" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="28"/>
+    </row>
+    <row r="105" spans="2:5">
+      <c r="B105" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5">
+      <c r="B106" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5">
+      <c r="B107" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5">
+      <c r="B108" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D108" s="2"/>
+      <c r="E108" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5">
+      <c r="B109" s="1"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="3"/>
+    </row>
+    <row r="110" spans="2:5">
+      <c r="B110" s="1"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="3"/>
+    </row>
+    <row r="111" spans="2:5">
+      <c r="B111" s="10"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="3"/>
+    </row>
+    <row r="112" spans="2:5">
+      <c r="B112" s="10"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="3"/>
+    </row>
+    <row r="113" spans="2:5">
+      <c r="B113" s="10"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="3"/>
+    </row>
+    <row r="114" spans="2:5">
+      <c r="B114" s="10"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="3"/>
+    </row>
+    <row r="115" spans="2:5">
+      <c r="B115" s="10"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="3"/>
+    </row>
+    <row r="116" spans="2:5">
+      <c r="B116" s="10"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="3"/>
+    </row>
+    <row r="117" spans="2:5">
+      <c r="B117" s="10"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="13"/>
+    </row>
+    <row r="118" spans="2:5" ht="17.25" thickBot="1">
+      <c r="B118" s="4"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="B104:E104"/>
     <mergeCell ref="B60:E60"/>
     <mergeCell ref="B51:E51"/>
     <mergeCell ref="B2:E2"/>

</xml_diff>